<commit_message>
Updates with working tests and vitals reports
</commit_message>
<xml_diff>
--- a/run/templates/Module_Template.xlsx
+++ b/run/templates/Module_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/phygbu_leeds_ac_uk/Documents/Documents/Programming/phas_vitals/run/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\phas_vitals\phas_vitals\run\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{888AF671-0EBB-4541-84A2-B7CADDE2B34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDED43D3-5F8D-40D8-9DC8-14998143D6C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479F2911-F28B-477F-BF68-394B3ED9324B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1692" yWindow="-108" windowWidth="29136" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="612" yWindow="-108" windowWidth="30216" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExamTemplate" sheetId="2" r:id="rId1"/>
@@ -1723,67 +1723,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_3020OM99" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1866,36 +1806,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1916,6 +1826,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFAFB1"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2228,7 +2145,7 @@
   <dimension ref="A1:AF298"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:Q280"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -17004,20 +16921,23 @@
   <mergeCells count="1">
     <mergeCell ref="T1:T6"/>
   </mergeCells>
-  <conditionalFormatting sqref="S17:S281">
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"P"</formula>
+  <conditionalFormatting sqref="E16:Q281">
+    <cfRule type="expression" dxfId="9" priority="6">
+      <formula>AND(NOT(ISBLANK($A16)),NOT(ISBLANK(E$12)),EXACT(E16,"P"))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"F"</formula>
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>AND(NOT(ISBLANK($A16)),NOT(ISBLANK(E$12)),EXACT(E16,"F"))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>AND(NOT(ISBLANK($A16)),NOT(ISBLANK(E$12)),ISBLANK(E16))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:Q280">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>""</formula>
+  <conditionalFormatting sqref="S16:S281">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>AND(NOT(ISBLANK($A16)),EXACT(S16,"P"))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"P"</formula>
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>AND(NOT(ISBLANK($A16)),EXACT(S16,"F"))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>